<commit_message>
Kapitel 'gesetzliche Umlagen' geschrieben.
</commit_message>
<xml_diff>
--- a/Mitarbeitertypen und deren Sozialversicherungen.xlsx
+++ b/Mitarbeitertypen und deren Sozialversicherungen.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D4448-7027-4C7A-B118-387C08854F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93C1D15-6867-42DF-9F4D-5A088CB0190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -620,17 +631,17 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>